<commit_message>
Ulteriore aggiornamento file report-checklist.xlsx
Ulteriore aggiornamento del file report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/1.0/report-checklist.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="473">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1801,11 +1801,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -1891,8 +1891,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1907,28 +1908,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1939,37 +1919,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1989,8 +1938,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2013,25 +2020,18 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2084,6 +2084,132 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2102,91 +2228,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2198,13 +2246,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2216,55 +2258,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2588,6 +2588,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2599,15 +2617,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2630,23 +2639,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2677,11 +2671,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2689,118 +2689,118 @@
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2809,28 +2809,28 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5782,11 +5782,9 @@
         <v>100</v>
       </c>
       <c r="J35" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="K35" s="37" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="K35" s="37"/>
       <c r="L35" s="37"/>
       <c r="M35" s="37" t="s">
         <v>54</v>
@@ -5843,11 +5841,9 @@
         <v>106</v>
       </c>
       <c r="J36" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="K36" s="37" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="K36" s="37"/>
       <c r="L36" s="37"/>
       <c r="M36" s="37" t="s">
         <v>54</v>
@@ -5904,11 +5900,9 @@
         <v>111</v>
       </c>
       <c r="J37" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="K37" s="37" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="K37" s="37"/>
       <c r="L37" s="37"/>
       <c r="M37" s="37" t="s">
         <v>54</v>
@@ -5965,11 +5959,9 @@
         <v>116</v>
       </c>
       <c r="J38" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="K38" s="37" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="K38" s="37"/>
       <c r="L38" s="37"/>
       <c r="M38" s="37" t="s">
         <v>54</v>
@@ -6026,11 +6018,9 @@
         <v>121</v>
       </c>
       <c r="J39" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="K39" s="37" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="K39" s="37"/>
       <c r="L39" s="37"/>
       <c r="M39" s="37" t="s">
         <v>54</v>
@@ -6087,11 +6077,9 @@
         <v>127</v>
       </c>
       <c r="J40" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="K40" s="37" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="K40" s="37"/>
       <c r="L40" s="37"/>
       <c r="M40" s="37" t="s">
         <v>54</v>
@@ -6148,11 +6136,9 @@
         <v>133</v>
       </c>
       <c r="J41" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="K41" s="37" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="K41" s="37"/>
       <c r="L41" s="37"/>
       <c r="M41" s="37" t="s">
         <v>54</v>
@@ -6209,11 +6195,9 @@
         <v>138</v>
       </c>
       <c r="J42" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="K42" s="37" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="K42" s="37"/>
       <c r="L42" s="37"/>
       <c r="M42" s="37" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Modifiche i file di test
Eseguiti nuovamente i test indicati
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/1.0/report-checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="12120" activeTab="2"/>
+    <workbookView windowWidth="29865" windowHeight="12000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -281,13 +281,13 @@
 </t>
   </si>
   <si>
-    <t>2025-05-09T09:03:37Z</t>
-  </si>
-  <si>
-    <t>40c955d249a28745a7d79bbd0418f258</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.9fea09c6bd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-16T12:00:56Z</t>
+  </si>
+  <si>
+    <t>0f509e4d059bd4fecb41fb454c2f7a4b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.02158f87a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -1589,13 +1589,13 @@
 </t>
   </si>
   <si>
-    <t>2025-05-09T09:15:20Z</t>
-  </si>
-  <si>
-    <t>241af028a1a86cf562547741689fa3bb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.e432ca63ea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-16T12:04:00Z</t>
+  </si>
+  <si>
+    <t>619e8a2fff9992c6c8114bf8794b72e2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.b0cf93cd19^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT30</t>
@@ -1842,10 +1842,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -1933,9 +1933,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1949,45 +1955,16 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1995,14 +1972,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2011,6 +1988,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2025,8 +2009,54 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2040,38 +2070,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2118,7 +2118,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2130,19 +2196,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2154,37 +2286,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2196,109 +2298,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2622,30 +2622,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2657,6 +2633,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2676,27 +2667,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2719,152 +2693,178 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4500,11 +4500,11 @@
   <dimension ref="A1:W755"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="O10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4533333333333" defaultRowHeight="15" customHeight="1"/>
@@ -4807,7 +4807,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="33">
-        <v>45786</v>
+        <v>45793</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>51</v>
@@ -11108,7 +11108,7 @@
         <v>409</v>
       </c>
       <c r="F173" s="35">
-        <v>45786</v>
+        <v>45793</v>
       </c>
       <c r="G173" s="35" t="s">
         <v>410</v>

</xml_diff>

<commit_message>
Modificato file del T4
Modifiche al file T4
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/1.0/report-checklist.xlsx
@@ -281,13 +281,13 @@
 </t>
   </si>
   <si>
-    <t>2025-05-21T17:02:46Z</t>
-  </si>
-  <si>
-    <t>72af06245609df790ab4838bbfaf7d8c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.ada818c981^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-22T13:48:23Z</t>
+  </si>
+  <si>
+    <t>e9f7d206a5ae691b5c2fe0bc0b92a83c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.a5d629f814^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -1841,11 +1841,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -1933,9 +1933,32 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1949,9 +1972,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1965,6 +2002,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1973,18 +2017,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1997,67 +2048,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2070,8 +2061,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2118,7 +2118,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2136,7 +2166,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2148,37 +2226,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2190,13 +2256,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2208,97 +2298,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2622,6 +2622,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2652,15 +2676,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2678,35 +2693,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2719,152 +2708,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4504,7 +4504,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H173" sqref="H173"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4533333333333" defaultRowHeight="15" customHeight="1"/>
@@ -4807,7 +4807,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="33">
-        <v>45798</v>
+        <v>45799</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>51</v>

</xml_diff>